<commit_message>
- new set of commands to support asynchronous web service or API invocation - refactor WS command and related code due to the introduction of async WS - fixed typos - migrated more code to Kotlin (SmsHelper, ExecutionEvent, SmsCommand, StepCommand) - widen event support beyond the existing 4 (start, complete, pause, error) - added multi-plan support.  Now it is possible to specify multiple plan files (no multiple plan-sheets support) - added usage tracking (experimental) -
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/step-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/step-showcase.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10516"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7A7637-4118-E240-977A-6EAC7C923CDB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F65166-1233-4F44-8CB8-60310C0D2ED9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20480" yWindow="440" windowWidth="20480" windowHeight="12580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31540" yWindow="-20560" windowWidth="11200" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -36,10 +36,15 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -571,7 +576,7 @@
   <dimension ref="A1:AAA10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>

</xml_diff>